<commit_message>
Added comparison sheet to feedback data
</commit_message>
<xml_diff>
--- a/Report/Resources/Feedback Data.xlsx
+++ b/Report/Resources/Feedback Data.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="2"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
     <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Non-Euclidean" sheetId="3" r:id="rId3"/>
+    <sheet name="NonEuclidean" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparison" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
   <si>
     <t>Experiment 1</t>
   </si>
@@ -249,6 +250,24 @@
   <si>
     <t>Comfort</t>
   </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Exp1</t>
+  </si>
+  <si>
+    <t>Exp2</t>
+  </si>
+  <si>
+    <t>Non-Euclidean</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,7 +841,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Comfort navigating standard scene</a:t>
+              <a:t> Comfort Navigating standard scene</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1280,7 +1300,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> of immersion related to navigation comfort in standard scene</a:t>
+              <a:t> of Immersion related to Navigation comfort in standard scene</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1326,7 +1346,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Standard!$C$25</c:f>
+              <c:f>Standard!$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1359,7 +1379,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Standard!$B$26:$B$35</c:f>
+              <c:f>Standard!$B$20:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1398,7 +1418,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Standard!$C$26:$C$35</c:f>
+              <c:f>Standard!$C$20:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1837,7 +1857,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Non-Euclidean'!$F$6:$O$6</c:f>
+              <c:f>NonEuclidean!$F$6:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2200,7 +2220,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Comfort navigating Non-Euclidean scene</a:t>
+              <a:t> Comfort Navigating Non-Euclidean scene</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2257,7 +2277,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Non-Euclidean'!$F$24:$O$24</c:f>
+              <c:f>NonEuclidean!$F$24:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2620,7 +2640,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> of immersion related to navigation comfort in Non-Euclidean scene</a:t>
+              <a:t> of Immersion related to Navigation comfort in Non-Euclidean scene</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2687,7 +2707,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Non-Euclidean'!$B$26:$B$35</c:f>
+              <c:f>NonEuclidean!$B$20:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2726,7 +2746,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Non-Euclidean'!$C$26:$C$35</c:f>
+              <c:f>NonEuclidean!$C$20:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3062,6 +3082,987 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Sense of Immersion between Standard and Non-Euclidean scenes in Experiment 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Standard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$B$20:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ABA3-4DF3-A441-2CFA643B3A7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non-Euclidean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$A$20:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ABA3-4DF3-A441-2CFA643B3A7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="417607552"/>
+        <c:axId val="417606240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="417607552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Participant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417606240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="417606240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sense of Immersion</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417607552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Sense of Immersion between Standard and Non-Euclidean scenes in Experiment 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Standard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E2D-445D-9828-68DF6BF0C95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non-Euclidean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1E2D-445D-9828-68DF6BF0C95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="417607552"/>
+        <c:axId val="417606240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="417607552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Participant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417606240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="417606240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sense of Immersion</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417607552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3302,6 +4303,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6327,6 +7408,1012 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6542,6 +8629,75 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7355,7 +9511,7 @@
   <dimension ref="A3:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7366,17 +9522,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F4" t="s">
         <v>72</v>
       </c>
@@ -7508,25 +9667,19 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <v>8</v>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -7545,46 +9698,90 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>6</v>
       </c>
       <c r="C15" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>7</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2">
+        <v>7</v>
+      </c>
       <c r="F22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2">
+        <v>8</v>
+      </c>
       <c r="F23">
         <v>1</v>
       </c>
@@ -7616,7 +9813,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
       <c r="F24">
         <v>0</v>
       </c>
@@ -7648,31 +9851,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2">
+        <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>6</v>
       </c>
@@ -7680,60 +9883,62 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <f>AVERAGE(B7,B9,B10,B13,B14,B15,B17)</f>
         <v>7</v>
       </c>
-      <c r="C30" s="2">
-        <v>5</v>
+      <c r="C33">
+        <f>AVERAGE(C7,C9,C10,C13,C14,C15,C17)</f>
+        <v>6.7142857142857144</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
-        <v>8</v>
-      </c>
-      <c r="C31" s="2">
-        <v>8</v>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <f>AVERAGE(B6,B8,B16)</f>
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <f>AVERAGE(C6,C8,C16)</f>
+        <v>7.666666666666667</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>8</v>
-      </c>
-      <c r="C32" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
-        <v>6</v>
-      </c>
-      <c r="C33" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>6</v>
-      </c>
-      <c r="C34" s="2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35">
+        <f>AVERAGE(B20:B29)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
+      <c r="C35">
+        <f>AVERAGE(C20:C29)</f>
         <v>7</v>
-      </c>
-      <c r="C35" s="2">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -7746,8 +9951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7758,17 +9963,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F4" t="s">
         <v>72</v>
       </c>
@@ -7900,25 +10108,19 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C12" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -7926,10 +10128,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -7937,40 +10139,87 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2">
         <v>7</v>
-      </c>
-      <c r="C14" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>7</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
       <c r="F22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6</v>
+      </c>
       <c r="F23">
         <v>1</v>
       </c>
@@ -8002,7 +10251,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4</v>
+      </c>
       <c r="F24">
         <v>0</v>
       </c>
@@ -8034,96 +10289,250 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2">
         <v>9</v>
       </c>
-      <c r="C26" s="2">
-        <v>9</v>
-      </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <f>AVERAGE(B7,B9,B10,B13,B14,B15,B17)</f>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="C33">
+        <f>AVERAGE(C7,C9,C10,C13,C14,C15,C17)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <f>AVERAGE(B6,B8,B16)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="C34">
+        <f>AVERAGE(C6,C8,C16)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35">
+        <f>AVERAGE(B20:B29)</f>
         <v>7</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
-        <v>8</v>
-      </c>
-      <c r="C30" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
-        <v>6</v>
-      </c>
-      <c r="C31" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>8</v>
-      </c>
-      <c r="C32" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
-        <v>7</v>
-      </c>
-      <c r="C33" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <v>7</v>
-      </c>
-      <c r="C35" s="2">
-        <v>9</v>
+      <c r="C35">
+        <f>AVERAGE(C20:C29)</f>
+        <v>6.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>Standard!B6</f>
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <f>NonEuclidean!B6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>Standard!B7</f>
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <f>NonEuclidean!B7</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>Standard!B8</f>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>NonEuclidean!B8</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>Standard!B9</f>
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>NonEuclidean!B9</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>Standard!B10</f>
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <f>NonEuclidean!B10</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>Standard!B13</f>
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <f>NonEuclidean!B13</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>Standard!B14</f>
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <f>NonEuclidean!B14</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>Standard!B15</f>
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <f>NonEuclidean!B15</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>Standard!B16</f>
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <f>NonEuclidean!B16</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>Standard!B17</f>
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <f>NonEuclidean!B17</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated feedback data spreadsheets
</commit_message>
<xml_diff>
--- a/Report/Resources/Feedback Data.xlsx
+++ b/Report/Resources/Feedback Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="3"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,12 @@
     <sheet name="NonEuclidean" sheetId="3" r:id="rId3"/>
     <sheet name="Comparison" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">(Comparison!$A$3:$A$7,Comparison!$A$20:$A$24)</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">(Comparison!$B$3:$B$7,Comparison!$B$20:$B$24)</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -517,7 +522,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FACC-462D-8D3D-5D6B8E2C293F}"/>
+              <c16:uniqueId val="{00000000-5E20-4FB7-976B-CADBDC0FF2B6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -976,7 +981,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FA74-4733-BA23-09AB877C7146}"/>
+              <c16:uniqueId val="{00000000-6008-40F9-8FE3-02F8ED31F26C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1458,7 +1463,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A6B8-4548-A283-C88BC7FF6039}"/>
+              <c16:uniqueId val="{00000000-B456-4C1C-A644-E6AAE93A5959}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1634,7 +1639,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Comfort</a:t>
+                  <a:t>Navigation Comfort</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2023,6 +2028,7 @@
         <c:axId val="409300688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2961,7 +2967,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Comfort</a:t>
+                  <a:t>Navigation Comfort</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3117,7 +3123,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Sense of Immersion between Standard and Non-Euclidean scenes in Experiment 2</a:t>
+              <a:t>Sense of Immersion between Standard and Non-Euclidean scenes in Experiment 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3159,11 +3165,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Comparison!$B$19</c:f>
+              <c:f>Comparison!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3184,21 +3190,21 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$B$20:$B$24</c:f>
+              <c:f>Comparison!$A$3:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7</c:v>
@@ -3208,16 +3214,16 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-ABA3-4DF3-A441-2CFA643B3A7C}"/>
+              <c16:uniqueId val="{00000000-1E2D-445D-9828-68DF6BF0C95B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Comparison!$A$19</c:f>
+              <c:f>Comparison!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3238,31 +3244,31 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$A$20:$A$24</c:f>
+              <c:f>Comparison!$B$3:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ABA3-4DF3-A441-2CFA643B3A7C}"/>
+              <c16:uniqueId val="{00000001-1E2D-445D-9828-68DF6BF0C95B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3312,6 +3318,522 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47765857392825894"/>
+              <c:y val="0.85553222513852434"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417606240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="417606240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sense of Immersion</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417607552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32851662292213474"/>
+          <c:y val="0.92187445319335082"/>
+          <c:w val="0.35407786526684165"/>
+          <c:h val="7.8125546806649168E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Sense of Immersion between Standard and Non-Euclidean scenes in Experiment 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Standard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$A$20:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5971-47E1-9E6E-F891A76F50DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non-Euclidean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$B$20:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5971-47E1-9E6E-F891A76F50DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="417607552"/>
+        <c:axId val="417606240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="417607552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Participant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47132524059492564"/>
+              <c:y val="0.86016185476815399"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3507,7 +4029,17 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3229610673665792"/>
+          <c:y val="0.92187445319335082"/>
+          <c:w val="0.35407786526684165"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3573,494 +4105,101 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Sense of Immersion between Standard and Non-Euclidean scenes in Experiment 1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Variation in Immersion</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
+          <a:pPr algn="ctr">
+            <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Variation in Immersion</a:t>
+          </a:r>
         </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Comparison!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Standard</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Comparison!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1E2D-445D-9828-68DF6BF0C95B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Comparison!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Non-Euclidean</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Comparison!$B$3:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1E2D-445D-9828-68DF6BF0C95B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="417607552"/>
-        <c:axId val="417606240"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="417607552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Participant</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{E55393AC-DA83-4629-903A-95CF9CB28BE6}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Standard</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-FDC9-4EF4-B34F-1A55B94019A7}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Non-Euclidean</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="1" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="0.150000006"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Immersion Rating</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
+              <a:pPr algn="ctr">
+                <a:defRPr/>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:r>
+                <a:rPr lang="en-US"/>
+                <a:t>Immersion Rating</a:t>
+              </a:r>
             </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="417606240"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="417606240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Sense of Immersion</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="417607552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4383,6 +4522,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -8429,6 +8608,492 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -8438,20 +9103,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8468,20 +9135,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8497,21 +9166,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8635,38 +9306,6 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -8689,10 +9328,114 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="9" name="Chart 8"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1924050" y="6286500"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8998,7 +9741,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9511,7 +10254,7 @@
   <dimension ref="A3:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9951,8 +10694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10389,8 +11132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10474,10 +11217,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed the scale on a few of the generated graphs
</commit_message>
<xml_diff>
--- a/Report/Resources/Feedback Data.xlsx
+++ b/Report/Resources/Feedback Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="2"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <definedName name="_xlchart.v2.1" hidden="1">(Comparison!$B$3:$B$7,Comparison!$B$20:$B$24)</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1482,6 +1481,7 @@
         <c:axId val="496154320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1601,6 +1601,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2811,6 +2812,7 @@
         <c:axId val="496154320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2929,6 +2931,7 @@
         <c:axId val="496147432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4172,7 +4175,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling min="1"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -10253,8 +10256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10694,8 +10697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11133,7 +11136,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Report formatting and misc fixes
* Further graph fixes

* Reworded Abstract

* Made fixes based on lit review feedback. Re-added multi-column support for entire report

* Completed intro for literature review. Misc formatting.
</commit_message>
<xml_diff>
--- a/Report/Resources/Feedback Data.xlsx
+++ b/Report/Resources/Feedback Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlchart.v2.1" hidden="1">(Comparison!$B$3:$B$7,Comparison!$B$20:$B$24)</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -375,7 +376,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>1-10 Sense</a:t>
+              <a:t>Sense</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -690,12 +691,20 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Occurences</a:t>
+                  <a:t> Occurrences</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.25874234470691165"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -840,12 +849,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>1-10</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Comfort Navigating standard scene</a:t>
+              <a:t>Comfort Navigating standard scene</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1150,7 +1155,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number of Occurences</a:t>
+                  <a:t>Number of Occurrences</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1795,7 +1800,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>1-10 Sense</a:t>
+              <a:t>Sense</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -2072,12 +2077,20 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Occurences</a:t>
+                  <a:t> Occurrences</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.26217993584135318"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2222,12 +2235,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>1-10</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Comfort Navigating Non-Euclidean scene</a:t>
+              <a:t>Comfort Navigating Non-Euclidean scene</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2493,7 +2502,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number of Occurences</a:t>
+                  <a:t>Number of Occurrences</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3406,6 +3415,7 @@
         <c:axId val="417606240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3915,6 +3925,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -10256,8 +10267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10698,7 +10709,7 @@
   <dimension ref="A3:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11135,8 +11146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated scatter graphs to include trend lines
</commit_message>
<xml_diff>
--- a/Report/Resources/Feedback Data.xlsx
+++ b/Report/Resources/Feedback Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="9300" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Consistent lighting/shoding felt like real flourescent indoor scenario. Corridor width also consistent like a real building interior</t>
   </si>
   <si>
     <t>The only control option to turn was a 45 degree angle snap that wasn't completely fluid, or as consistent as the fluidity of the movement</t>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>STD DEV</t>
+  </si>
+  <si>
+    <t>Consistent lighting/shading felt like real flourescent indoor scenario. Corridor width also consistent like a real building interior</t>
   </si>
 </sst>
 </file>
@@ -1388,6 +1388,52 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0.5"/>
+            <c:backward val="1"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Standard!$B$20:$B$29</c:f>
@@ -2723,6 +2769,22 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0.5"/>
+            <c:backward val="1"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>NonEuclidean!$B$20:$B$29</c:f>
@@ -9757,7 +9819,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9817,37 +9879,37 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="2">
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2">
         <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="K3" s="2">
         <v>9</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -9858,37 +9920,37 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="2">
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2">
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="K4" s="2">
         <v>6</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -9899,37 +9961,37 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="2">
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2">
         <v>7</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="K5" s="2">
         <v>5</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -9940,37 +10002,37 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="2">
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2">
         <v>6</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="2">
         <v>6</v>
       </c>
       <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -9981,37 +10043,37 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2">
         <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="K7" s="2">
         <v>4</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -10065,37 +10127,37 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="2">
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="2">
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="K11" s="2">
         <v>8</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -10106,37 +10168,37 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E12" s="2">
         <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="2">
         <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="K12" s="2">
         <v>8</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -10147,37 +10209,37 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="2">
         <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="2">
         <v>5</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -10188,37 +10250,37 @@
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E14" s="2">
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="2">
         <v>6</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="K14" s="2">
         <v>7</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -10229,34 +10291,34 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2">
         <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2">
         <v>7</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="K15" s="2">
         <v>10</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -10269,8 +10331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10282,21 +10344,21 @@
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -10427,7 +10489,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -10501,10 +10563,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
         <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -10531,7 +10593,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -10652,13 +10714,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -10689,7 +10751,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <f>AVERAGE(B20:B29)</f>
@@ -10702,10 +10764,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -10729,7 +10791,7 @@
   <dimension ref="A3:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10741,21 +10803,21 @@
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -10886,7 +10948,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -10957,10 +11019,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
         <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -10987,7 +11049,7 @@
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -11108,13 +11170,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -11145,7 +11207,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <f>AVERAGE(B20:B29)</f>
@@ -11158,10 +11220,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -11195,18 +11257,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11261,18 +11323,18 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Completed analysis of non-Euclidean scene experiment results
</commit_message>
<xml_diff>
--- a/Report/Resources/Feedback Data.xlsx
+++ b/Report/Resources/Feedback Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -280,7 +280,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +292,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +333,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1402,37 +1412,7 @@
             <c:forward val="0.5"/>
             <c:backward val="1"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -9819,7 +9799,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10331,8 +10311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10788,10 +10768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O37"/>
+  <dimension ref="A3:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11179,7 +11159,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -11192,7 +11172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -11205,7 +11185,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -11218,7 +11198,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -11226,7 +11206,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B37">
         <f>_xlfn.STDEV.P(B6,B7,B8,B9,B10,B13,B14,B15,B16,B17)</f>
         <v>1.3416407864998738</v>
@@ -11235,6 +11215,7 @@
         <f>_xlfn.STDEV.P(C6,C7,C8,C9,C10,C13,C14,C15,C16,C17)</f>
         <v>1.6</v>
       </c>
+      <c r="R37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>